<commit_message>
Foi adicionado farois na plahnilha feedback para que possamos indentificar os itens que precissamos trabalhar
</commit_message>
<xml_diff>
--- a/--Feedbacks--/FeedBack Sprint 1.xlsx
+++ b/--Feedbacks--/FeedBack Sprint 1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dbbbc15b312a8d85/Documentos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dbbbc15b312a8d85/sptech/Sp-tech/Ads2/LP/lista-03-metodos-PedroHPCSouza-1/Área de Trabalho/NocTotamento/Documentacao/--Feedbacks--/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1C671335-38A0-4F44-B267-09BD26F61CAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="62" documentId="8_{1C671335-38A0-4F44-B267-09BD26F61CAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6775D07F-87A2-4A45-A9C6-D4528D77B2D9}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{180F2781-2C27-4193-866D-DFED58236500}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>ITEM DE AVALIAÇÃO</t>
   </si>
@@ -116,12 +116,27 @@
     <t xml:space="preserve">	
 inovação - não ficou claro na apresentação onde este item vai estar implementado...</t>
   </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>LEGENDA</t>
+  </si>
+  <si>
+    <t>Em Risco</t>
+  </si>
+  <si>
+    <t>EM Andamento</t>
+  </si>
+  <si>
+    <t>Concluido</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,8 +167,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -175,6 +197,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -206,7 +246,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -224,6 +264,21 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -558,94 +613,123 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD0F5D7E-F96E-470D-B6E1-97B92E80DE16}">
-  <dimension ref="B2:F11"/>
+  <dimension ref="B2:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="28.28515625" customWidth="1"/>
     <col min="3" max="3" width="119" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="2:6" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D3" s="7"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="13"/>
+    </row>
+    <row r="4" spans="2:10" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="2:6" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D4" s="7"/>
+    </row>
+    <row r="5" spans="2:10" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D5" s="8"/>
+    </row>
+    <row r="6" spans="2:10" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D6" s="7"/>
+    </row>
+    <row r="7" spans="2:10" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="2:6" ht="119.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D7" s="7"/>
+    </row>
+    <row r="8" spans="2:10" ht="119.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="D8" s="7"/>
       <c r="F8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="147" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" ht="147" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="7"/>
+    </row>
+    <row r="10" spans="2:10" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D10" s="12"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>

</xml_diff>